<commit_message>
cleaned up python script
</commit_message>
<xml_diff>
--- a/testfile.xlsx
+++ b/testfile.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14780" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="2018-12-29-bbs-listings" sheetId="5" r:id="rId1"/>
+    <sheet name="biz-listings" sheetId="5" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="dh_bbs_harvested_data" localSheetId="0">'2018-12-29-bbs-listings'!$A$1:$H$13</definedName>
+    <definedName name="dh_bbs_harvested_data" localSheetId="0">'biz-listings'!$A$1:$H$13</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -714,7 +714,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>